<commit_message>
feat: add Usecase_Scenarios and Planification_initiale in pdf
</commit_message>
<xml_diff>
--- a/Pré-TPI_Journal_de_Travail.xlsx
+++ b/Pré-TPI_Journal_de_Travail.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eduvaud-my.sharepoint.com/personal/pv22nbo_eduvaud_ch/Documents/Bureau/Pré-TPI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="48" documentId="8_{5332EB15-E1EF-46C3-9C5F-7D49BA9E428F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B31DADD2-3223-4736-A188-B415D5AA95E6}"/>
+  <xr:revisionPtr revIDLastSave="87" documentId="8_{5332EB15-E1EF-46C3-9C5F-7D49BA9E428F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E44A17E-C699-44E9-B4F8-4C2F08436985}"/>
   <bookViews>
-    <workbookView xWindow="3990" yWindow="2310" windowWidth="21600" windowHeight="11295" xr2:uid="{2D24A8E9-E825-4E48-9C88-9BFF47DB70A1}"/>
+    <workbookView xWindow="-1365" yWindow="1215" windowWidth="21600" windowHeight="11295" xr2:uid="{2D24A8E9-E825-4E48-9C88-9BFF47DB70A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de Travail" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Date</t>
   </si>
@@ -81,6 +81,45 @@
   </si>
   <si>
     <t>Fait avec Gantt project</t>
+  </si>
+  <si>
+    <t>35 min</t>
+  </si>
+  <si>
+    <t>Continuation de la planification du projet</t>
+  </si>
+  <si>
+    <t>Finalisation de la planification du projet</t>
+  </si>
+  <si>
+    <t>Fin de la Planification du projet</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Début de la Planification Initiale du projet</t>
+  </si>
+  <si>
+    <t>Création des Use cases</t>
+  </si>
+  <si>
+    <t>Aide avec Gemini pour les Use cases</t>
+  </si>
+  <si>
+    <t>30 min</t>
+  </si>
+  <si>
+    <t>Scenarios</t>
+  </si>
+  <si>
+    <t>Les scénarios sont créent dans le même fichier que les use cases</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50 min </t>
+  </si>
+  <si>
+    <t>Création du MCD</t>
+  </si>
+  <si>
+    <t>LE MCD est créer avec draw.io</t>
   </si>
 </sst>
 </file>
@@ -137,11 +176,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -166,6 +204,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -488,13 +530,13 @@
   <dimension ref="B5:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="61.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -513,10 +555,10 @@
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>46055</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -527,10 +569,10 @@
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="5">
+      <c r="B7" s="4">
         <v>46055</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -541,10 +583,10 @@
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="5">
+      <c r="B8" s="4">
         <v>46055</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -555,153 +597,193 @@
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="5">
+      <c r="B9" s="4">
         <v>46055</v>
       </c>
-      <c r="C9" s="3">
-        <v>0.67013888888888884</v>
+      <c r="C9" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="6"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+      <c r="B10" s="4">
+        <v>46056</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="6"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
+      <c r="B11" s="4">
+        <v>46056</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="6"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
+      <c r="B12" s="4">
+        <v>46056</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="6"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
+      <c r="B13" s="4">
+        <v>46056</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="6"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="B14" s="4">
+        <v>46056</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.65277777777777779</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="6"/>
+      <c r="B15" s="5"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="6"/>
+      <c r="B16" s="5"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="6"/>
+      <c r="B17" s="5"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="6"/>
+      <c r="B18" s="5"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="6"/>
+      <c r="B19" s="5"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="6"/>
+      <c r="B20" s="5"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="6"/>
+      <c r="B21" s="5"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="6"/>
+      <c r="B22" s="5"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="6"/>
+      <c r="B23" s="5"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="6"/>
+      <c r="B24" s="5"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="6"/>
+      <c r="B25" s="5"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="6"/>
+      <c r="B26" s="5"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="6"/>
+      <c r="B27" s="5"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="6"/>
+      <c r="B28" s="5"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="6"/>
+      <c r="B29" s="5"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="6"/>
+      <c r="B30" s="5"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="6"/>
+      <c r="B31" s="5"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="6"/>
+      <c r="B32" s="5"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>

</xml_diff>

<commit_message>
feat: ajout du  MCD et mis a jour du Journal_de_travail
</commit_message>
<xml_diff>
--- a/Pré-TPI_Journal_de_Travail.xlsx
+++ b/Pré-TPI_Journal_de_Travail.xlsx
@@ -8,12 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eduvaud-my.sharepoint.com/personal/pv22nbo_eduvaud_ch/Documents/Bureau/Pré-TPI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="87" documentId="8_{5332EB15-E1EF-46C3-9C5F-7D49BA9E428F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E44A17E-C699-44E9-B4F8-4C2F08436985}"/>
+  <xr:revisionPtr revIDLastSave="140" documentId="8_{5332EB15-E1EF-46C3-9C5F-7D49BA9E428F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{753A4B97-77C1-4A0A-9B9B-0D5F0A27AACD}"/>
   <bookViews>
-    <workbookView xWindow="-1365" yWindow="1215" windowWidth="21600" windowHeight="11295" xr2:uid="{2D24A8E9-E825-4E48-9C88-9BFF47DB70A1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2D24A8E9-E825-4E48-9C88-9BFF47DB70A1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Journal de Travail" sheetId="1" r:id="rId1"/>
+    <sheet name="Semaine 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Semaine 2" sheetId="2" r:id="rId2"/>
+    <sheet name="Semaine 3" sheetId="3" r:id="rId3"/>
+    <sheet name="Semaine 4" sheetId="4" r:id="rId4"/>
+    <sheet name="Semaine 5" sheetId="5" r:id="rId5"/>
+    <sheet name="Semaine 6" sheetId="6" r:id="rId6"/>
+    <sheet name="Semaine 7" sheetId="7" r:id="rId7"/>
+    <sheet name="Semaine 8" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="32">
   <si>
     <t>Date</t>
   </si>
@@ -120,6 +127,18 @@
   </si>
   <si>
     <t>LE MCD est créer avec draw.io</t>
+  </si>
+  <si>
+    <t>MCD</t>
+  </si>
+  <si>
+    <t>Continuation et Fin du MCD</t>
+  </si>
+  <si>
+    <t>Amélioration de la Partie 1 du doc</t>
+  </si>
+  <si>
+    <t>16:00 à 16:35</t>
   </si>
 </sst>
 </file>
@@ -530,7 +549,7 @@
   <dimension ref="B5:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -681,110 +700,1983 @@
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="5"/>
-      <c r="C15" s="1"/>
+      <c r="B15" s="4">
+        <v>46057</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0.66597222222222219</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="4">
+        <v>46057</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4075700A-7AA2-495E-BBE0-C6F5E0E70C3A}">
+  <dimension ref="B5:E32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="5" width="38.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="59" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="4"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="4"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="4"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="4"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="4"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="4"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="4"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="4"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="4"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="4"/>
+      <c r="C15" s="3"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="5"/>
-      <c r="C16" s="1"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="3"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="5"/>
-      <c r="C17" s="1"/>
+      <c r="C17" s="5"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="5"/>
-      <c r="C18" s="1"/>
+      <c r="C18" s="5"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="5"/>
-      <c r="C19" s="1"/>
+      <c r="C19" s="5"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="5"/>
-      <c r="C20" s="1"/>
+      <c r="C20" s="5"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="5"/>
-      <c r="C21" s="1"/>
+      <c r="C21" s="5"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="5"/>
-      <c r="C22" s="1"/>
+      <c r="C22" s="5"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="5"/>
-      <c r="C23" s="1"/>
+      <c r="C23" s="5"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="5"/>
-      <c r="C24" s="1"/>
+      <c r="C24" s="5"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="5"/>
-      <c r="C25" s="1"/>
+      <c r="C25" s="5"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="5"/>
-      <c r="C26" s="1"/>
+      <c r="C26" s="5"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="5"/>
-      <c r="C27" s="1"/>
+      <c r="C27" s="5"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="5"/>
-      <c r="C28" s="1"/>
+      <c r="C28" s="5"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="5"/>
-      <c r="C29" s="1"/>
+      <c r="C29" s="5"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="5"/>
-      <c r="C30" s="1"/>
+      <c r="C30" s="5"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" s="5"/>
-      <c r="C31" s="1"/>
+      <c r="C31" s="5"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" s="5"/>
-      <c r="C32" s="1"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F35A02E-1228-4FE0-AB52-0B7DF9AA1E26}">
+  <dimension ref="B5:E32"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="4">
+        <v>46055</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="4">
+        <v>46055</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="4">
+        <v>46055</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="4">
+        <v>46055</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="4">
+        <v>46056</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="4">
+        <v>46056</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="4">
+        <v>46056</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="4">
+        <v>46056</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="4">
+        <v>46056</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.65277777777777779</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="4">
+        <v>46057</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0.66597222222222219</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="4">
+        <v>46057</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16DF8FDC-C826-4B60-A93B-FDAF95CDC872}">
+  <dimension ref="B5:E32"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="4">
+        <v>46055</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="4">
+        <v>46055</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="4">
+        <v>46055</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="4">
+        <v>46055</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="4">
+        <v>46056</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="4">
+        <v>46056</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="4">
+        <v>46056</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="4">
+        <v>46056</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="4">
+        <v>46056</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.65277777777777779</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="4">
+        <v>46057</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0.66597222222222219</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="4">
+        <v>46057</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B2363BD-8413-4FBE-8016-B2A5DD09713E}">
+  <dimension ref="B5:E32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="4">
+        <v>46055</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="4">
+        <v>46055</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="4">
+        <v>46055</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="4">
+        <v>46055</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="4">
+        <v>46056</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="4">
+        <v>46056</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="4">
+        <v>46056</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="4">
+        <v>46056</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="4">
+        <v>46056</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.65277777777777779</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="4">
+        <v>46057</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0.66597222222222219</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="4">
+        <v>46057</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C30B61C-8412-4C43-8E38-33998CF51391}">
+  <dimension ref="B5:E32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="4">
+        <v>46055</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="4">
+        <v>46055</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="4">
+        <v>46055</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="4">
+        <v>46055</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="4">
+        <v>46056</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="4">
+        <v>46056</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="4">
+        <v>46056</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="4">
+        <v>46056</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="4">
+        <v>46056</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.65277777777777779</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="4">
+        <v>46057</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0.66597222222222219</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="4">
+        <v>46057</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF7254E8-1FC7-423F-BF9B-1683B3423B85}">
+  <dimension ref="B5:E32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="4">
+        <v>46055</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="4">
+        <v>46055</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="4">
+        <v>46055</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="4">
+        <v>46055</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="4">
+        <v>46056</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="4">
+        <v>46056</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="4">
+        <v>46056</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="4">
+        <v>46056</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="4">
+        <v>46056</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.65277777777777779</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="4">
+        <v>46057</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0.66597222222222219</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="4">
+        <v>46057</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6F65FA1-77F3-4CDB-AB7D-E59545EF6CD0}">
+  <dimension ref="B5:E32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="4">
+        <v>46055</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="4">
+        <v>46055</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="4">
+        <v>46055</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="4">
+        <v>46055</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="4">
+        <v>46056</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="4">
+        <v>46056</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="4">
+        <v>46056</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="4">
+        <v>46056</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="4">
+        <v>46056</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.65277777777777779</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="4">
+        <v>46057</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0.66597222222222219</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="4">
+        <v>46057</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
     </row>

</xml_diff>

<commit_message>
refactor: MAJ du MCD et du journal de travail + ajout diagramme de classes
</commit_message>
<xml_diff>
--- a/Pré-TPI_Journal_de_Travail.xlsx
+++ b/Pré-TPI_Journal_de_Travail.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eduvaud-my.sharepoint.com/personal/pv22nbo_eduvaud_ch/Documents/Bureau/Pré-TPI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="140" documentId="8_{5332EB15-E1EF-46C3-9C5F-7D49BA9E428F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{753A4B97-77C1-4A0A-9B9B-0D5F0A27AACD}"/>
+  <xr:revisionPtr revIDLastSave="172" documentId="8_{5332EB15-E1EF-46C3-9C5F-7D49BA9E428F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0D43EA02-5EBA-4B04-8888-C0727009408A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2D24A8E9-E825-4E48-9C88-9BFF47DB70A1}"/>
+    <workbookView xWindow="1785" yWindow="1350" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{2D24A8E9-E825-4E48-9C88-9BFF47DB70A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Semaine 1" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="45">
   <si>
     <t>Date</t>
   </si>
@@ -139,6 +139,45 @@
   </si>
   <si>
     <t>16:00 à 16:35</t>
+  </si>
+  <si>
+    <t>Maquettes</t>
+  </si>
+  <si>
+    <t>Utilisation de Figma pour les maquettes</t>
+  </si>
+  <si>
+    <t>40 min</t>
+  </si>
+  <si>
+    <t>Création du MLD</t>
+  </si>
+  <si>
+    <t>Avec MySQL Workbench</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Modification du MCD</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ajout d'Identifiant naturels</t>
+  </si>
+  <si>
+    <t>Fin du MLD</t>
+  </si>
+  <si>
+    <t>Finalisation du MLD</t>
+  </si>
+  <si>
+    <t>Diagramme de Classes</t>
+  </si>
+  <si>
+    <t>Création du Diagramme UML</t>
+  </si>
+  <si>
+    <t>Fin du Diagramme de Classes</t>
+  </si>
+  <si>
+    <t>Finalisation du Diagramme UML</t>
   </si>
 </sst>
 </file>
@@ -546,10 +585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09C44FD8-239F-4390-A2A6-95504ADCF907}">
-  <dimension ref="B5:E32"/>
+  <dimension ref="B5:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -727,102 +766,6 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -832,8 +775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4075700A-7AA2-495E-BBE0-C6F5E0E70C3A}">
   <dimension ref="B5:E32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -857,40 +800,88 @@
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="4"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
+      <c r="B6" s="4">
+        <v>46062</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="4"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
+      <c r="B7" s="4">
+        <v>46062</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.59444444444444444</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="4"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+      <c r="B8" s="4">
+        <v>46062</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="4"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+      <c r="B9" s="4">
+        <v>46062</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.63888888888888884</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="4"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+      <c r="B10" s="4">
+        <v>46062</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.64236111111111116</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="4"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
+      <c r="B11" s="4">
+        <v>46062</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="4"/>

</xml_diff>